<commit_message>
update correcciones y tc pe44
</commit_message>
<xml_diff>
--- a/test_cases/PE-16.xlsx
+++ b/test_cases/PE-16.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="88">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t>Additional information = Big windLorem ipsum dolor sit amet, consectetur adipiscing elit. Vivamus varius, ex eu elementum gravida, mauris nisi scelerisque quam, tempor dapibus orci quam ultricies lacus. Suspendisse dapibus, nibh sed pharetra accumsan, dolor ligula varius ante, a rutrum justo mi fringilla nunc. Lorem ipsum dolor sit amet, consectetur adipiscing elit. Duis dui velit, commodo vel lectus in, mollis porta elit. Quisque interdum leo purus, vitae fringilla risus tincidunt quis. Pellentesque fringilla nisi quis diam  owed building on the corner.A</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -794,107 +800,164 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -902,67 +965,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1251,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8:K8"/>
     </sheetView>
   </sheetViews>
@@ -1274,19 +1280,19 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="G1" s="43" t="s">
+      <c r="E1" s="47"/>
+      <c r="G1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
@@ -1298,24 +1304,24 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50"/>
+      <c r="E2" s="61"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="3" spans="1:14" ht="22.5">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
@@ -1326,10 +1332,10 @@
       <c r="G3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="53"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="18" t="s">
         <v>14</v>
       </c>
@@ -1358,14 +1364,14 @@
       <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34" t="s">
+      <c r="I5" s="65"/>
+      <c r="J5" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="35"/>
+      <c r="K5" s="67"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -1374,14 +1380,14 @@
       <c r="G6" s="22">
         <v>1</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="37" t="s">
+      <c r="I6" s="70"/>
+      <c r="J6" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="12" t="s">
@@ -1399,14 +1405,14 @@
       <c r="G7" s="22">
         <v>2</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="37" t="s">
+      <c r="I7" s="70"/>
+      <c r="J7" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="70"/>
     </row>
     <row r="8" spans="1:14" ht="22.5">
       <c r="A8" s="15">
@@ -1424,14 +1430,14 @@
       <c r="G8" s="22">
         <v>3</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="37" t="s">
+      <c r="I8" s="70"/>
+      <c r="J8" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="38"/>
+      <c r="K8" s="70"/>
     </row>
     <row r="9" spans="1:14" ht="22.5">
       <c r="A9" s="15">
@@ -1494,16 +1500,16 @@
       <c r="E14" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
     </row>
     <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="D15" s="17">
@@ -1512,22 +1518,22 @@
       <c r="E15" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36" t="s">
+      <c r="H15" s="68"/>
+      <c r="I15" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36" t="s">
+      <c r="J15" s="68"/>
+      <c r="K15" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36" t="s">
+      <c r="L15" s="68"/>
+      <c r="M15" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="36"/>
+      <c r="N15" s="68"/>
     </row>
     <row r="16" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="D16" s="17">
@@ -1536,22 +1542,22 @@
       <c r="E16" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="30" t="s">
+      <c r="H16" s="63"/>
+      <c r="I16" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="30" t="s">
+      <c r="J16" s="63"/>
+      <c r="K16" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="30" t="s">
+      <c r="L16" s="63"/>
+      <c r="M16" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="31"/>
+      <c r="N16" s="63"/>
     </row>
     <row r="17" spans="4:14" ht="39" thickTop="1">
       <c r="D17" s="17">
@@ -1708,84 +1714,101 @@
       <c r="N23" s="16"/>
     </row>
     <row r="25" spans="4:14">
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29" t="s">
+      <c r="H25" s="71"/>
+      <c r="I25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29" t="s">
+      <c r="J25" s="71"/>
+      <c r="K25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29" t="s">
+      <c r="L25" s="71"/>
+      <c r="M25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="29"/>
+      <c r="N25" s="71"/>
     </row>
     <row r="26" spans="4:14" ht="32.25" customHeight="1">
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28" t="s">
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
     </row>
     <row r="27" spans="4:14">
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
     </row>
     <row r="28" spans="4:14">
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
     </row>
     <row r="29" spans="4:14">
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
     </row>
     <row r="30" spans="4:14">
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:K2"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
@@ -1802,30 +1825,13 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:K2"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1854,19 +1860,19 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="G1" s="43" t="s">
+      <c r="E1" s="47"/>
+      <c r="G1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
@@ -1878,22 +1884,22 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50"/>
+      <c r="E2" s="74"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="3" spans="1:14" ht="22.5">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
@@ -1904,10 +1910,10 @@
       <c r="G3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="53"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="18" t="s">
         <v>14</v>
       </c>
@@ -1936,14 +1942,14 @@
       <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34" t="s">
+      <c r="I5" s="65"/>
+      <c r="J5" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="35"/>
+      <c r="K5" s="67"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -1952,14 +1958,14 @@
       <c r="G6" s="22">
         <v>1</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="37" t="s">
+      <c r="I6" s="70"/>
+      <c r="J6" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="12" t="s">
@@ -1977,14 +1983,14 @@
       <c r="G7" s="22">
         <v>2</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="37" t="s">
+      <c r="I7" s="70"/>
+      <c r="J7" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="70"/>
     </row>
     <row r="8" spans="1:14" ht="54" customHeight="1">
       <c r="A8" s="15">
@@ -2002,14 +2008,14 @@
       <c r="G8" s="22">
         <v>3</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="37" t="s">
+      <c r="I8" s="70"/>
+      <c r="J8" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="38"/>
+      <c r="K8" s="70"/>
     </row>
     <row r="9" spans="1:14" ht="22.5">
       <c r="A9" s="15">
@@ -2072,16 +2078,16 @@
       <c r="E14" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
     </row>
     <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="D15" s="17">
@@ -2090,22 +2096,22 @@
       <c r="E15" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36" t="s">
+      <c r="H15" s="68"/>
+      <c r="I15" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36" t="s">
+      <c r="J15" s="68"/>
+      <c r="K15" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36" t="s">
+      <c r="L15" s="68"/>
+      <c r="M15" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="36"/>
+      <c r="N15" s="68"/>
     </row>
     <row r="16" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="D16" s="17">
@@ -2114,22 +2120,22 @@
       <c r="E16" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="30" t="s">
+      <c r="H16" s="63"/>
+      <c r="I16" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="30" t="s">
+      <c r="J16" s="63"/>
+      <c r="K16" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="30" t="s">
+      <c r="L16" s="63"/>
+      <c r="M16" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="31"/>
+      <c r="N16" s="63"/>
     </row>
     <row r="17" spans="4:14" ht="39" thickTop="1">
       <c r="D17" s="17">
@@ -2286,77 +2292,111 @@
       <c r="N23" s="16"/>
     </row>
     <row r="25" spans="4:14">
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29" t="s">
+      <c r="H25" s="71"/>
+      <c r="I25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29" t="s">
+      <c r="J25" s="71"/>
+      <c r="K25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29" t="s">
+      <c r="L25" s="71"/>
+      <c r="M25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="29"/>
+      <c r="N25" s="71"/>
     </row>
     <row r="26" spans="4:14">
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28" t="s">
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
     </row>
     <row r="27" spans="4:14">
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
     </row>
     <row r="28" spans="4:14">
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
     </row>
     <row r="29" spans="4:14">
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
     </row>
     <row r="30" spans="4:14">
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="G1:G2"/>
@@ -2370,40 +2410,6 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2432,19 +2438,19 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="G1" s="43" t="s">
+      <c r="E1" s="47"/>
+      <c r="G1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
@@ -2456,24 +2462,24 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50"/>
+      <c r="E2" s="61"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="3" spans="1:14" ht="22.5">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
@@ -2484,10 +2490,10 @@
       <c r="G3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="53"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="18" t="s">
         <v>14</v>
       </c>
@@ -2516,14 +2522,14 @@
       <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34" t="s">
+      <c r="I5" s="65"/>
+      <c r="J5" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="35"/>
+      <c r="K5" s="67"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -2532,14 +2538,14 @@
       <c r="G6" s="22">
         <v>1</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="37" t="s">
+      <c r="I6" s="70"/>
+      <c r="J6" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="12" t="s">
@@ -2557,14 +2563,14 @@
       <c r="G7" s="22">
         <v>2</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="37" t="s">
+      <c r="I7" s="70"/>
+      <c r="J7" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="70"/>
     </row>
     <row r="8" spans="1:14" ht="55.5" customHeight="1">
       <c r="A8" s="15">
@@ -2582,14 +2588,14 @@
       <c r="G8" s="22">
         <v>3</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="37" t="s">
+      <c r="I8" s="70"/>
+      <c r="J8" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="38"/>
+      <c r="K8" s="70"/>
     </row>
     <row r="9" spans="1:14" ht="22.5">
       <c r="A9" s="15">
@@ -2652,16 +2658,16 @@
       <c r="E14" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
     </row>
     <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="D15" s="17">
@@ -2670,22 +2676,22 @@
       <c r="E15" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36" t="s">
+      <c r="H15" s="68"/>
+      <c r="I15" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36" t="s">
+      <c r="J15" s="68"/>
+      <c r="K15" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36" t="s">
+      <c r="L15" s="68"/>
+      <c r="M15" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="36"/>
+      <c r="N15" s="68"/>
     </row>
     <row r="16" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="D16" s="17">
@@ -2694,22 +2700,22 @@
       <c r="E16" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="30" t="s">
+      <c r="H16" s="63"/>
+      <c r="I16" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="30" t="s">
+      <c r="J16" s="63"/>
+      <c r="K16" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="30" t="s">
+      <c r="L16" s="63"/>
+      <c r="M16" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="31"/>
+      <c r="N16" s="63"/>
     </row>
     <row r="17" spans="4:14" ht="39" thickTop="1">
       <c r="D17" s="17">
@@ -2866,94 +2872,92 @@
       <c r="N23" s="16"/>
     </row>
     <row r="25" spans="4:14">
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29" t="s">
+      <c r="H25" s="71"/>
+      <c r="I25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29" t="s">
+      <c r="J25" s="71"/>
+      <c r="K25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29" t="s">
+      <c r="L25" s="71"/>
+      <c r="M25" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="29"/>
+      <c r="N25" s="71"/>
     </row>
     <row r="26" spans="4:14">
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28" t="s">
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
     </row>
     <row r="27" spans="4:14">
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
     </row>
     <row r="28" spans="4:14">
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
     </row>
     <row r="29" spans="4:14">
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
     </row>
     <row r="30" spans="4:14">
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:K2"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="K27:L27"/>
@@ -2968,22 +2972,24 @@
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="M16:N16"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
     <mergeCell ref="M15:N15"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:K2"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2994,7 +3000,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3007,408 +3013,408 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="29.25" customHeight="1">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="43" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="22.5">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="67" t="s">
+      <c r="B3" s="83"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="69"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="53"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="60"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="31"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
     </row>
     <row r="5" spans="1:14" ht="33.75">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+        <v>87</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34" t="s">
+      <c r="I5" s="65"/>
+      <c r="J5" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
     </row>
     <row r="6" spans="1:14" ht="32.25" customHeight="1">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="71">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="38">
         <v>1</v>
       </c>
-      <c r="H6" s="72" t="s">
+      <c r="H6" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="72" t="s">
+      <c r="I6" s="79"/>
+      <c r="J6" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="75" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="71">
+      <c r="F7" s="31"/>
+      <c r="G7" s="38">
         <v>2</v>
       </c>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="72" t="s">
+      <c r="I7" s="79"/>
+      <c r="J7" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="73"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
     </row>
     <row r="8" spans="1:14" ht="22.5">
       <c r="A8" s="23">
         <v>1</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="60"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="24">
         <v>1</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="60"/>
-      <c r="G8" s="71">
+      <c r="F8" s="31"/>
+      <c r="G8" s="38">
         <v>3</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="73"/>
-      <c r="J8" s="72" t="s">
+      <c r="I8" s="79"/>
+      <c r="J8" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="73"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
     </row>
     <row r="9" spans="1:14" ht="22.5">
       <c r="A9" s="23">
         <v>2</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="24">
         <v>2</v>
       </c>
-      <c r="E9" s="77" t="s">
+      <c r="E9" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
     </row>
     <row r="10" spans="1:14" ht="67.5">
       <c r="A10" s="23">
         <v>3</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="60"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="24">
         <v>3</v>
       </c>
-      <c r="E10" s="77" t="s">
+      <c r="E10" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="24">
         <v>4</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E11" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="24">
         <v>5</v>
       </c>
-      <c r="E12" s="77" t="s">
+      <c r="E12" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="24">
         <v>6</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="69"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
     </row>
     <row r="14" spans="1:14" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="24">
         <v>7</v>
       </c>
-      <c r="E14" s="77" t="s">
+      <c r="E14" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="60"/>
-      <c r="G14" s="78" t="s">
+      <c r="F14" s="31"/>
+      <c r="G14" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="78"/>
-      <c r="N14" s="78"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
     </row>
     <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A15" s="60"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="24">
         <v>8</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="36" t="s">
+      <c r="F15" s="31"/>
+      <c r="G15" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36" t="s">
+      <c r="H15" s="68"/>
+      <c r="I15" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36" t="s">
+      <c r="J15" s="68"/>
+      <c r="K15" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36" t="s">
+      <c r="L15" s="68"/>
+      <c r="M15" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="36"/>
+      <c r="N15" s="68"/>
     </row>
     <row r="16" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A16" s="60"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="24">
         <v>9</v>
       </c>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="60"/>
-      <c r="G16" s="79" t="s">
+      <c r="F16" s="31"/>
+      <c r="G16" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="80"/>
-      <c r="I16" s="79" t="s">
+      <c r="H16" s="76"/>
+      <c r="I16" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="80"/>
-      <c r="K16" s="79" t="s">
+      <c r="J16" s="76"/>
+      <c r="K16" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="80"/>
-      <c r="M16" s="79" t="s">
+      <c r="L16" s="76"/>
+      <c r="M16" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="80"/>
+      <c r="N16" s="76"/>
     </row>
     <row r="17" spans="1:14" ht="39" thickTop="1">
-      <c r="A17" s="60"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="24">
         <v>10</v>
       </c>
-      <c r="E17" s="77" t="s">
+      <c r="E17" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="60"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="21" t="s">
         <v>26</v>
       </c>
@@ -3435,16 +3441,16 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="60"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="24">
         <v>11</v>
       </c>
-      <c r="E18" s="77" t="s">
+      <c r="E18" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="60"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="23" t="s">
         <v>29</v>
       </c>
@@ -3469,16 +3475,16 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="225">
-      <c r="A19" s="60"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="24">
         <v>12</v>
       </c>
-      <c r="E19" s="77" t="s">
+      <c r="E19" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="60"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="23" t="s">
         <v>29</v>
       </c>
@@ -3503,16 +3509,16 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="60"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="24">
         <v>13</v>
       </c>
-      <c r="E20" s="77" t="s">
+      <c r="E20" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="60"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="23" t="s">
         <v>29</v>
       </c>
@@ -3537,177 +3543,212 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="60"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="77"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="42"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="60"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="77"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="77"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="42"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="60"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="77"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="42"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="60"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="60"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="84" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84" t="s">
+      <c r="H25" s="77"/>
+      <c r="I25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="84"/>
-      <c r="K25" s="84" t="s">
+      <c r="J25" s="77"/>
+      <c r="K25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="84"/>
-      <c r="M25" s="84" t="s">
+      <c r="L25" s="77"/>
+      <c r="M25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="84"/>
+      <c r="N25" s="77"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="60"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="60"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="60"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="60"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="60"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:K2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="K30:L30"/>
@@ -3720,41 +3761,6 @@
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:K2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3765,7 +3771,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3778,408 +3784,408 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34.5" customHeight="1">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="43" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="22.5">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="67" t="s">
+      <c r="B3" s="83"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="69"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="53"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="60"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="31"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
     </row>
     <row r="5" spans="1:14" ht="33.75">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+        <v>86</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34" t="s">
+      <c r="I5" s="65"/>
+      <c r="J5" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
     </row>
     <row r="6" spans="1:14" ht="31.5" customHeight="1">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="71">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="38">
         <v>1</v>
       </c>
-      <c r="H6" s="72" t="s">
+      <c r="H6" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="72" t="s">
+      <c r="I6" s="79"/>
+      <c r="J6" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="75" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="71">
+      <c r="F7" s="31"/>
+      <c r="G7" s="38">
         <v>2</v>
       </c>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="72" t="s">
+      <c r="I7" s="79"/>
+      <c r="J7" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="73"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
     </row>
     <row r="8" spans="1:14" ht="22.5">
       <c r="A8" s="23">
         <v>1</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="60"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="24">
         <v>1</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="60"/>
-      <c r="G8" s="71">
+      <c r="F8" s="31"/>
+      <c r="G8" s="38">
         <v>3</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="73"/>
-      <c r="J8" s="72" t="s">
+      <c r="I8" s="79"/>
+      <c r="J8" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="73"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
     </row>
     <row r="9" spans="1:14" ht="22.5">
       <c r="A9" s="23">
         <v>2</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="24">
         <v>2</v>
       </c>
-      <c r="E9" s="77" t="s">
+      <c r="E9" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
     </row>
     <row r="10" spans="1:14" ht="67.5">
       <c r="A10" s="23">
         <v>3</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="60"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="24">
         <v>3</v>
       </c>
-      <c r="E10" s="77" t="s">
+      <c r="E10" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="24">
         <v>4</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E11" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="24">
         <v>5</v>
       </c>
-      <c r="E12" s="77" t="s">
+      <c r="E12" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="24">
         <v>6</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="69"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
     </row>
     <row r="14" spans="1:14" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="24">
         <v>7</v>
       </c>
-      <c r="E14" s="77" t="s">
+      <c r="E14" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="60"/>
-      <c r="G14" s="78" t="s">
+      <c r="F14" s="31"/>
+      <c r="G14" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="78"/>
-      <c r="N14" s="78"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
     </row>
     <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A15" s="60"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="24">
         <v>8</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="36" t="s">
+      <c r="F15" s="31"/>
+      <c r="G15" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36" t="s">
+      <c r="H15" s="68"/>
+      <c r="I15" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36" t="s">
+      <c r="J15" s="68"/>
+      <c r="K15" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36" t="s">
+      <c r="L15" s="68"/>
+      <c r="M15" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="36"/>
+      <c r="N15" s="68"/>
     </row>
     <row r="16" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A16" s="60"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="24">
         <v>9</v>
       </c>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="60"/>
-      <c r="G16" s="79" t="s">
+      <c r="F16" s="31"/>
+      <c r="G16" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="80"/>
-      <c r="I16" s="79" t="s">
+      <c r="H16" s="76"/>
+      <c r="I16" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="80"/>
-      <c r="K16" s="79" t="s">
+      <c r="J16" s="76"/>
+      <c r="K16" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="80"/>
-      <c r="M16" s="79" t="s">
+      <c r="L16" s="76"/>
+      <c r="M16" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="80"/>
+      <c r="N16" s="76"/>
     </row>
     <row r="17" spans="1:14" ht="39" thickTop="1">
-      <c r="A17" s="60"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="24">
         <v>10</v>
       </c>
-      <c r="E17" s="77" t="s">
+      <c r="E17" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="60"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="21" t="s">
         <v>26</v>
       </c>
@@ -4206,16 +4212,16 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="60"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="24">
         <v>11</v>
       </c>
-      <c r="E18" s="77" t="s">
+      <c r="E18" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="60"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="23" t="s">
         <v>29</v>
       </c>
@@ -4240,16 +4246,16 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="225">
-      <c r="A19" s="60"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="24">
         <v>12</v>
       </c>
-      <c r="E19" s="77" t="s">
+      <c r="E19" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="60"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="23" t="s">
         <v>29</v>
       </c>
@@ -4274,16 +4280,16 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="60"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="24">
         <v>13</v>
       </c>
-      <c r="E20" s="77" t="s">
+      <c r="E20" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="60"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="23" t="s">
         <v>29</v>
       </c>
@@ -4308,177 +4314,212 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="60"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="77"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="42"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="60"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="77"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="77"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="42"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="60"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="77"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="42"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="60"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="60"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="84" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84" t="s">
+      <c r="H25" s="77"/>
+      <c r="I25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="84"/>
-      <c r="K25" s="84" t="s">
+      <c r="J25" s="77"/>
+      <c r="K25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="84"/>
-      <c r="M25" s="84" t="s">
+      <c r="L25" s="77"/>
+      <c r="M25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="84"/>
+      <c r="N25" s="77"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="60"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="60"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="60"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="60"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="60"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:K2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="K30:L30"/>
@@ -4491,41 +4532,6 @@
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:K2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4535,8 +4541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4549,408 +4555,408 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="33" customHeight="1">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="43" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="22.5">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="67" t="s">
+      <c r="B3" s="83"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="69"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="53"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="60"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="31"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
     </row>
     <row r="5" spans="1:14" ht="33.75">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+        <v>86</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34" t="s">
+      <c r="I5" s="65"/>
+      <c r="J5" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
     </row>
     <row r="6" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="71">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="38">
         <v>1</v>
       </c>
-      <c r="H6" s="72" t="s">
+      <c r="H6" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="72" t="s">
+      <c r="I6" s="79"/>
+      <c r="J6" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="75" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="71">
+      <c r="F7" s="31"/>
+      <c r="G7" s="38">
         <v>2</v>
       </c>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="72" t="s">
+      <c r="I7" s="79"/>
+      <c r="J7" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="73"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
     </row>
     <row r="8" spans="1:14" ht="22.5">
       <c r="A8" s="23">
         <v>1</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="60"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="24">
         <v>1</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="60"/>
-      <c r="G8" s="71">
+      <c r="F8" s="31"/>
+      <c r="G8" s="38">
         <v>3</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="73"/>
-      <c r="J8" s="72" t="s">
+      <c r="I8" s="79"/>
+      <c r="J8" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="73"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
     </row>
     <row r="9" spans="1:14" ht="22.5">
       <c r="A9" s="23">
         <v>2</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="24">
         <v>2</v>
       </c>
-      <c r="E9" s="77" t="s">
+      <c r="E9" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
     </row>
     <row r="10" spans="1:14" ht="67.5">
       <c r="A10" s="23">
         <v>3</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="60"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="24">
         <v>3</v>
       </c>
-      <c r="E10" s="77" t="s">
+      <c r="E10" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="24">
         <v>4</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E11" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="24">
         <v>5</v>
       </c>
-      <c r="E12" s="77" t="s">
+      <c r="E12" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="24">
         <v>6</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="69"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
     </row>
     <row r="14" spans="1:14" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="24">
         <v>7</v>
       </c>
-      <c r="E14" s="77" t="s">
+      <c r="E14" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="60"/>
-      <c r="G14" s="78" t="s">
+      <c r="F14" s="31"/>
+      <c r="G14" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="78"/>
-      <c r="N14" s="78"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
     </row>
     <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A15" s="60"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="24">
         <v>8</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="36" t="s">
+      <c r="F15" s="31"/>
+      <c r="G15" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36" t="s">
+      <c r="H15" s="68"/>
+      <c r="I15" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36" t="s">
+      <c r="J15" s="68"/>
+      <c r="K15" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36" t="s">
+      <c r="L15" s="68"/>
+      <c r="M15" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="36"/>
+      <c r="N15" s="68"/>
     </row>
     <row r="16" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A16" s="60"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="24">
         <v>9</v>
       </c>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="60"/>
-      <c r="G16" s="79" t="s">
+      <c r="F16" s="31"/>
+      <c r="G16" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="80"/>
-      <c r="I16" s="79" t="s">
+      <c r="H16" s="76"/>
+      <c r="I16" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="80"/>
-      <c r="K16" s="79" t="s">
+      <c r="J16" s="76"/>
+      <c r="K16" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="80"/>
-      <c r="M16" s="79" t="s">
+      <c r="L16" s="76"/>
+      <c r="M16" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="80"/>
+      <c r="N16" s="76"/>
     </row>
     <row r="17" spans="1:14" ht="39" thickTop="1">
-      <c r="A17" s="60"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="24">
         <v>10</v>
       </c>
-      <c r="E17" s="77" t="s">
+      <c r="E17" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="60"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="21" t="s">
         <v>26</v>
       </c>
@@ -4977,16 +4983,16 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="60"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="24">
         <v>11</v>
       </c>
-      <c r="E18" s="77" t="s">
+      <c r="E18" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="60"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="23" t="s">
         <v>29</v>
       </c>
@@ -5011,16 +5017,16 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="225">
-      <c r="A19" s="60"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="24">
         <v>12</v>
       </c>
-      <c r="E19" s="77" t="s">
+      <c r="E19" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="60"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="23" t="s">
         <v>29</v>
       </c>
@@ -5045,16 +5051,16 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="60"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="24">
         <v>13</v>
       </c>
-      <c r="E20" s="77" t="s">
+      <c r="E20" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="60"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="23" t="s">
         <v>29</v>
       </c>
@@ -5079,177 +5085,212 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="60"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="77"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="42"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="60"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="77"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="77"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="42"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="60"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="77"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="42"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="60"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="60"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="84" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84" t="s">
+      <c r="H25" s="77"/>
+      <c r="I25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="84"/>
-      <c r="K25" s="84" t="s">
+      <c r="J25" s="77"/>
+      <c r="K25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="84"/>
-      <c r="M25" s="84" t="s">
+      <c r="L25" s="77"/>
+      <c r="M25" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="84"/>
+      <c r="N25" s="77"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="60"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="60"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="60"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="60"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="60"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:K2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="K30:L30"/>
@@ -5262,41 +5303,6 @@
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="M29:N29"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:K2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>